<commit_message>
Enable SELL trading. FIxed lots of bugs and configurations for SELL trades to work.
</commit_message>
<xml_diff>
--- a/Bot_config.xlsx
+++ b/Bot_config.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Algos\git\binance-spot-bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konstantin\Desktop\pythonProjects\binance-spot-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37D9CC7-8FB9-4C21-8684-2DC97613343F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="46290" windowHeight="25410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Validity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>symbol</t>
   </si>
@@ -55,9 +54,6 @@
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>USDT</t>
-  </si>
-  <si>
     <t>BUY</t>
   </si>
   <si>
@@ -67,18 +63,12 @@
     <t>LMT</t>
   </si>
   <si>
-    <t xml:space="preserve">BTC </t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
     <t>SELL</t>
   </si>
   <si>
-    <t>Currently owned position size</t>
-  </si>
-  <si>
     <t>Open positions limit</t>
   </si>
   <si>
@@ -623,15 +613,12 @@
   </si>
   <si>
     <t>ETHUSDT</t>
-  </si>
-  <si>
-    <t>ETH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -766,28 +753,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,29 +1036,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="56" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.44140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="3" customWidth="1"/>
-    <col min="11" max="1025" width="9.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="3" customWidth="1"/>
+    <col min="11" max="1025" width="9.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1097,197 +1084,207 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="3">
         <v>100</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="F3" s="3">
+        <v>100</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="10" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="12" spans="1:8" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="18"/>
-    </row>
-    <row r="14" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+    <row r="16" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+    <row r="17" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+    <row r="18" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1297,33 +1294,31 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+    <row r="20" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+    <row r="21" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+    <row r="22" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="18"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1331,122 +1326,111 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+    <row r="23" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="29" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="32" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="15"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:F30"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1456,23 +1440,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validity!$D$2:$D$16</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D5 B10</xm:sqref>
+          <xm:sqref>B8 D2:D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validity!$E$2:$E$3</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E2:E5</xm:sqref>
+          <xm:sqref>E2:E3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1481,29 +1465,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="3" width="9.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1529,108 +1513,108 @@
         <v>7</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="J2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J3" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor bot logic to support SPOT trading, allow for proper order management and execute trades accordingly to the plan.
</commit_message>
<xml_diff>
--- a/Bot_config.xlsx
+++ b/Bot_config.xlsx
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1196,9 +1196,8 @@
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="B6" s="7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>